<commit_message>
giảm bớt connect khi lưu dữ liệu, còn học phần nữa tối làm
</commit_message>
<xml_diff>
--- a/uploads/Điền thông tin GV mời KTMT 29102024(Sheet1)1 - Copy.xlsx
+++ b/uploads/Điền thông tin GV mời KTMT 29102024(Sheet1)1 - Copy.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>STT</t>
   </si>
@@ -66,66 +66,6 @@
     <t>Ngân hàng Techcombank</t>
   </si>
   <si>
-    <t>n.d.thang1987@gmail.com</t>
-  </si>
-  <si>
-    <t>NEC Vietnam Co Ltd.</t>
-  </si>
-  <si>
-    <t>19/04/2018</t>
-  </si>
-  <si>
-    <t>13/9/1986</t>
-  </si>
-  <si>
-    <t>thanhvanbkhn@gmail.com</t>
-  </si>
-  <si>
-    <t>Ngân hàng VP Bank</t>
-  </si>
-  <si>
-    <t>Ngân hàng TMCP VP Bank</t>
-  </si>
-  <si>
-    <t>23/09/1978</t>
-  </si>
-  <si>
-    <t>phanminhnhuvp@gmail.com</t>
-  </si>
-  <si>
-    <t>Ngân hàng VietinBank – chi nhánh Phúc Yên</t>
-  </si>
-  <si>
-    <t>thuanpv89@gmail.com</t>
-  </si>
-  <si>
-    <t>20/11/1998</t>
-  </si>
-  <si>
-    <t>anhnguyen981102@gmail.com</t>
-  </si>
-  <si>
-    <t>21/11/1998</t>
-  </si>
-  <si>
-    <t>docongminh8888@gmail.com</t>
-  </si>
-  <si>
-    <t>CMC TS</t>
-  </si>
-  <si>
-    <t>18/09/2024</t>
-  </si>
-  <si>
-    <t>MBBank, Phúc La</t>
-  </si>
-  <si>
-    <t>hoangcongtuyen271299@gmail.com</t>
-  </si>
-  <si>
-    <t>29/11/2016</t>
-  </si>
-  <si>
     <t>Họ và tên</t>
   </si>
   <si>
@@ -198,82 +138,7 @@
     <t>Tổ 2 Tân Hòa, thành phố Hòa Bình, Hòa Bình</t>
   </si>
   <si>
-    <t>Quản lý</t>
-  </si>
-  <si>
-    <t>P910HH2D KĐT mới Dương nội, Yên Nghĩa, Hà Đông, Hà Nội</t>
-  </si>
-  <si>
-    <t>Ngân hàng TMCP Kỹ thương việt nam (techcombank), chi nhánh Hoàng Quốc Việt</t>
-  </si>
-  <si>
-    <t>Nữ</t>
-  </si>
-  <si>
-    <t>Kiến trúc sư hệ thống</t>
-  </si>
-  <si>
-    <t>Thôn Nhị Trai, Trừng Xá, Lương Tài, Bắc Ninh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trường Đại học Công nghệ GTVT </t>
-  </si>
-  <si>
-    <t>TDP Tân Tiến, Tích Sơn, Thành phố Vĩnh Yên, Vĩnh Phúc</t>
-  </si>
-  <si>
-    <t>216 B2TT GVĐH CN TVTV, Thanh Xuân Nam, T/Xuân, Hà Nội</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ngân hàng Quốc tế VIB – chi nhánh Hai Bà Trưng </t>
-  </si>
-  <si>
-    <t>GV thỉnh giảng</t>
-  </si>
-  <si>
-    <t>Học viện KTMM</t>
-  </si>
-  <si>
-    <t>Số nhà 176, thôn Việt Long, Tản Lĩnh, Ba Vì, Hà Nội</t>
-  </si>
-  <si>
-    <t>Ngân hàng TMCP Ngoại thương Việt Nam (VCB), chi nhánh Nam Từ Liêm</t>
-  </si>
-  <si>
-    <t>Xa La, Hà Đông, Hà Nội</t>
-  </si>
-  <si>
-    <t>Thực tập</t>
-  </si>
-  <si>
-    <t>Xã Song Giang, huyện Gia Bình, tỉnh Bắc Ninh</t>
-  </si>
-  <si>
-    <t>viecombank,Bắc Ninh</t>
-  </si>
-  <si>
     <t>Nguyễn Thanh Sơn nay</t>
-  </si>
-  <si>
-    <t>Nguyễn Đức Thắng nay</t>
-  </si>
-  <si>
-    <t>Lý Thị Thanh Vân nay</t>
-  </si>
-  <si>
-    <t>Phan Như Minh nay</t>
-  </si>
-  <si>
-    <t>Phùng Văn Thuần nay</t>
-  </si>
-  <si>
-    <t>Nguyễn Hồng Anh nay</t>
-  </si>
-  <si>
-    <t>Đỗ Công Minh nay</t>
-  </si>
-  <si>
-    <t>Hoàng Công Tuyên nay</t>
   </si>
   <si>
     <t>Nguyễn Minh Tuấn nay</t>
@@ -1194,15 +1059,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="12" max="12" width="38.1796875" customWidth="1"/>
+    <col min="12" max="12" width="58.08984375" customWidth="1"/>
     <col min="13" max="13" width="18.1796875" customWidth="1"/>
     <col min="16" max="16" width="15" customWidth="1"/>
   </cols>
@@ -1212,61 +1077,61 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="S1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="165">
@@ -1274,7 +1139,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>4</v>
@@ -1289,31 +1154,31 @@
         <v>7</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="J2" s="5">
         <v>4.4000000000000004</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="L2" s="5">
-        <v>1226075003834</v>
+        <v>1.23523260750038E+16</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="P2" s="5">
         <v>8053747985</v>
@@ -1322,7 +1187,7 @@
         <v>42610000097218</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="S2" s="9" t="s">
         <v>5</v>
@@ -1336,7 +1201,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>4</v>
@@ -1351,7 +1216,7 @@
         <v>11</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>8</v>
@@ -1363,7 +1228,7 @@
         <v>3</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="L3" s="5">
         <v>1217094007872</v>
@@ -1372,10 +1237,10 @@
         <v>13</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="P3" s="5">
         <v>8139038927</v>
@@ -1390,445 +1255,12 @@
         <v>5</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" ht="231">
-      <c r="A4" s="4">
-        <v>4</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="6">
-        <v>31848</v>
-      </c>
-      <c r="E4" s="5">
-        <v>977954458</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="J4" s="5">
-        <v>4</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="5">
-        <v>1237087003636</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="P4" s="5">
-        <v>8095590888</v>
-      </c>
-      <c r="Q4" s="5">
-        <v>11722307021010</v>
-      </c>
-      <c r="R4" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="S4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="T4" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="148.5">
-      <c r="A5" s="4">
-        <v>5</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="5">
-        <v>987629720</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="J5" s="5">
-        <v>3.99</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="L5" s="5">
-        <v>1233186014693</v>
-      </c>
-      <c r="M5" s="6">
-        <v>44542</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="P5" s="5">
-        <v>8103250006</v>
-      </c>
-      <c r="Q5" s="5">
-        <v>260231097</v>
-      </c>
-      <c r="R5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="S5" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="T5" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" ht="181.5">
-      <c r="A6" s="4">
-        <v>6</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="5">
-        <v>912979207</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="J6" s="5">
-        <v>4</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="L6" s="5">
-        <v>1226078001538</v>
-      </c>
-      <c r="M6" s="6">
-        <v>44473</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="P6" s="5">
-        <v>8072856122</v>
-      </c>
-      <c r="Q6" s="5">
-        <v>106003983584</v>
-      </c>
-      <c r="R6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="S6" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="T6" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" ht="181.5">
-      <c r="A7" s="4">
-        <v>7</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="6">
-        <v>32569</v>
-      </c>
-      <c r="E7" s="5">
-        <v>989923698</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="J7" s="5">
-        <v>4</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="L7" s="5">
-        <v>1236089000558</v>
-      </c>
-      <c r="M7" s="6">
-        <v>44870</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="O7" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="P7" s="5">
-        <v>8319454690</v>
-      </c>
-      <c r="Q7" s="5">
-        <v>4704060067454</v>
-      </c>
-      <c r="R7" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="S7" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="T7" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" ht="214.5">
-      <c r="A8" s="4">
-        <v>8</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="5">
-        <v>865256498</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J8" s="5">
-        <v>2.34</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="L8" s="5">
-        <v>109800747712</v>
-      </c>
-      <c r="M8" s="6">
-        <v>44903</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5">
-        <v>1029289578</v>
-      </c>
-      <c r="R8" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="S8" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="T8" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" ht="82.5">
-      <c r="A9" s="4">
-        <v>9</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="5">
-        <v>868546800</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J9" s="5">
-        <v>2.34</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L9" s="5">
-        <v>1236098015186</v>
-      </c>
-      <c r="M9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="N9" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="O9" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5">
-        <v>56003686</v>
-      </c>
-      <c r="R9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="S9" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="T9" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" ht="148.5">
-      <c r="A10" s="4">
-        <v>11</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="6">
-        <v>36192</v>
-      </c>
-      <c r="E10" s="5">
-        <v>565646868</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="J10" s="5">
-        <v>2.34</v>
-      </c>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5">
-        <v>12125903419</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="N10" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="O10" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5">
-        <v>9965894442</v>
-      </c>
-      <c r="R10" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="S10" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="T10" s="9" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" display="mailto:tuannm1610@gmail.com"/>
-    <hyperlink ref="F4" r:id="rId2" display="mailto:n.d.thang1987@gmail.com"/>
-    <hyperlink ref="F5" r:id="rId3" display="mailto:thanhvanbkhn@gmail.com"/>
-    <hyperlink ref="F6" r:id="rId4" display="mailto:phanminhnhuvp@gmail.com"/>
-    <hyperlink ref="F7" r:id="rId5" display="mailto:thuanpv89@gmail.com"/>
-    <hyperlink ref="F8" r:id="rId6" display="mailto:anhnguyen981102@gmail.com"/>
-    <hyperlink ref="F9" r:id="rId7" display="mailto:docongminh8888@gmail.com"/>
-    <hyperlink ref="F10" r:id="rId8" display="mailto:hoangcongtuyen271299@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update thêm bộ môn cho gvm
</commit_message>
<xml_diff>
--- a/uploads/Điền thông tin GV mời KTMT 29102024(Sheet1)1 - Copy.xlsx
+++ b/uploads/Điền thông tin GV mời KTMT 29102024(Sheet1)1 - Copy.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="137">
   <si>
     <t>STT</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Nam</t>
   </si>
   <si>
-    <t>Khá</t>
-  </si>
-  <si>
     <t>Họ và tên</t>
   </si>
   <si>
@@ -90,173 +87,356 @@
     <t>Giảng viên</t>
   </si>
   <si>
-    <t>CCSĐKQLCTVDLQGVDC</t>
-  </si>
-  <si>
     <t>Thạc sĩ</t>
   </si>
   <si>
-    <t>Học viện Tài chính</t>
-  </si>
-  <si>
-    <t>Công ty TNHH phần mềm FPT</t>
-  </si>
-  <si>
-    <t>21/12/1980</t>
-  </si>
-  <si>
-    <t>chungphamdinh@gmail.com</t>
-  </si>
-  <si>
-    <t>Phạm Đình Chung</t>
-  </si>
-  <si>
-    <t>CA TP Hà Nội</t>
-  </si>
-  <si>
-    <t>14/80 Lê Trọng Tấn, Thanh Xuân, Hà Nội</t>
-  </si>
-  <si>
-    <t>Ngân hàng BIDV, chi nhánh Hà Thành, Hà Nội</t>
-  </si>
-  <si>
-    <t>DTVT</t>
-  </si>
-  <si>
-    <t>Nguyễn Thế Truyện</t>
-  </si>
-  <si>
-    <t>23/4/1964</t>
-  </si>
-  <si>
-    <t>truyennt6868@gmail.com</t>
-  </si>
-  <si>
-    <t>Viện trưởng</t>
-  </si>
-  <si>
-    <t>29/2/2016</t>
-  </si>
-  <si>
-    <t>Trần Anh Dũng</t>
-  </si>
-  <si>
-    <t>Đinh Văn Tuân</t>
-  </si>
-  <si>
-    <t>Đinh Nho Thanh</t>
-  </si>
-  <si>
-    <t>Đặng Trần Chuyên</t>
-  </si>
-  <si>
-    <t>21/06/1986</t>
-  </si>
-  <si>
-    <t>18/9/1957</t>
-  </si>
-  <si>
-    <t>23/4/1966</t>
-  </si>
-  <si>
-    <t>0989290754</t>
-  </si>
-  <si>
-    <t>0912095442</t>
-  </si>
-  <si>
-    <t>0984210686</t>
-  </si>
-  <si>
-    <t>0947365469</t>
-  </si>
-  <si>
-    <t>0389363125</t>
-  </si>
-  <si>
-    <t>0903433199</t>
-  </si>
-  <si>
-    <t>trananhdung21@gmail.com</t>
-  </si>
-  <si>
-    <t>Tiến sĩ</t>
-  </si>
-  <si>
-    <t>Giám đốc</t>
-  </si>
-  <si>
-    <t>Phó giám đốc</t>
-  </si>
-  <si>
-    <t>Nghỉ hưu</t>
-  </si>
-  <si>
-    <t>026080000033</t>
-  </si>
-  <si>
-    <t>027064000071</t>
-  </si>
-  <si>
-    <t>031057006770</t>
-  </si>
-  <si>
-    <t>001066011844</t>
-  </si>
-  <si>
-    <t>15/3/2018</t>
-  </si>
-  <si>
-    <t>Cục Cảnh Sát ĐKQL Cư trú và DLQG về Dân cư</t>
-  </si>
-  <si>
-    <t>0011000453665</t>
-  </si>
-  <si>
-    <t>22010000744116</t>
-  </si>
-  <si>
-    <t>0020149984004</t>
-  </si>
-  <si>
-    <t>11521988293018</t>
-  </si>
-  <si>
-    <t>Ngân hàng Techcombank, chi nhánh Ngọc Khánh, Hà Nội.</t>
-  </si>
-  <si>
-    <t>Ngân hàng Quân đội, chi nhánh hội sở chính</t>
-  </si>
-  <si>
-    <t>Ngân hàng BIDV</t>
-  </si>
-  <si>
-    <t>Ngân hàng quân đội MB. Chi nhánh MB Trần Duy Hưng</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ngân hàng TMCP Ngoại thương </t>
-  </si>
-  <si>
-    <t>Số 25 ngõ 42 Trần Cung, Cổ Nhuế, Bắc Từ Liêm, Hà Nội</t>
-  </si>
-  <si>
-    <t>P410, A12, Kim Giang - Thanh Xuân - Hà Nội</t>
-  </si>
-  <si>
-    <t>P 2707 Tòa E Tòa nhà  Mulberry Lane, Mộ  Lao, Hà Đông, Hà Nội</t>
-  </si>
-  <si>
-    <t>P1122 HH1C Linh Đàm, Hoàng Liệt, Hoàng Mai, Hà Nội</t>
-  </si>
-  <si>
-    <t>Căn A2102 Chung cư Hồng Kong, 243A Đê La Thành, Phường Láng Thượng, Quận Đống Đa Hà Nội</t>
+    <t>Nguyễn Thị Thanh Tâm</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Tới</t>
+  </si>
+  <si>
+    <t>Đặng Thị Kim Anh</t>
+  </si>
+  <si>
+    <t>Bùi Văn Công</t>
+  </si>
+  <si>
+    <t>Bùi Thị Như</t>
+  </si>
+  <si>
+    <t>Trịnh Anh Tuấn</t>
+  </si>
+  <si>
+    <t>Đỗ Bảo Sơn</t>
+  </si>
+  <si>
+    <t>Lê Thanh Tấn</t>
+  </si>
+  <si>
+    <t>Nguyễn Hưng Long</t>
+  </si>
+  <si>
+    <t>Nguyễn Thái Sơn</t>
+  </si>
+  <si>
+    <t>Trịnh Thị Xuân</t>
+  </si>
+  <si>
+    <t>Khuất Thị Ngọc Ánh</t>
+  </si>
+  <si>
+    <t>Nữ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04/08/2022        </t>
+  </si>
+  <si>
+    <t>Cục QLHC về trật tự xã hội</t>
+  </si>
+  <si>
+    <t>024079016540</t>
+  </si>
+  <si>
+    <t>04/08/2022</t>
+  </si>
+  <si>
+    <t>001182007087</t>
+  </si>
+  <si>
+    <t>07/04/2015</t>
+  </si>
+  <si>
+    <t>036083007024</t>
+  </si>
+  <si>
+    <t>30/04/2021</t>
+  </si>
+  <si>
+    <t>034185001956</t>
+  </si>
+  <si>
+    <t>02/08/2022</t>
+  </si>
+  <si>
+    <t>034083012886</t>
+  </si>
+  <si>
+    <t>031091011464</t>
+  </si>
+  <si>
+    <t>02/06/2020</t>
+  </si>
+  <si>
+    <t>030079009486</t>
+  </si>
+  <si>
+    <t>29/03/2021</t>
+  </si>
+  <si>
+    <t>001069003204</t>
+  </si>
+  <si>
+    <t>24/6/2021</t>
+  </si>
+  <si>
+    <t>042081016692</t>
+  </si>
+  <si>
+    <t>08/01/2022</t>
+  </si>
+  <si>
+    <t>038179013948</t>
+  </si>
+  <si>
+    <t>07/04/2021</t>
+  </si>
+  <si>
+    <t>001196016484</t>
+  </si>
+  <si>
+    <t>14/06/2022</t>
+  </si>
+  <si>
+    <t>0973002640</t>
+  </si>
+  <si>
+    <t>0867536913</t>
+  </si>
+  <si>
+    <t>0904876082</t>
+  </si>
+  <si>
+    <t>0983978015</t>
+  </si>
+  <si>
+    <t>0936507189</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0919200290 </t>
+  </si>
+  <si>
+    <t>0332336863</t>
+  </si>
+  <si>
+    <t>0912345399</t>
+  </si>
+  <si>
+    <t>0979734899</t>
+  </si>
+  <si>
+    <t>0969880912</t>
+  </si>
+  <si>
+    <t>0982083232</t>
+  </si>
+  <si>
+    <t>0392120967</t>
+  </si>
+  <si>
+    <t>ttvancntt@gmai.com</t>
+  </si>
+  <si>
+    <t>kimanh0602@gmail.com</t>
+  </si>
+  <si>
+    <t>bvcoong@gmail.com</t>
+  </si>
+  <si>
+    <t>nhubt1983@gmail.com</t>
+  </si>
+  <si>
+    <t>txtuan@gmail.com</t>
+  </si>
+  <si>
+    <t>sondb19@gmail.com</t>
+  </si>
+  <si>
+    <t>thanhtanhd@gmail.com</t>
+  </si>
+  <si>
+    <t>longtmu@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> thaison.nguyenn@gmail.com</t>
+  </si>
+  <si>
+    <t>trinhxuan@gmail.com</t>
+  </si>
+  <si>
+    <t>anhktn@utt.edu.vn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiến sỹ    </t>
+  </si>
+  <si>
+    <t>Nghiên cứu viên</t>
+  </si>
+  <si>
+    <t>Giảng viên chính</t>
+  </si>
+  <si>
+    <t>3.85</t>
+  </si>
+  <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>3.99</t>
+  </si>
+  <si>
+    <t>3.66</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>6.1</t>
+  </si>
+  <si>
+    <t>2.67</t>
+  </si>
+  <si>
+    <t>19036428472018</t>
+  </si>
+  <si>
+    <t>19033849649015</t>
+  </si>
+  <si>
+    <t>019704060203270</t>
+  </si>
+  <si>
+    <t>11121651434010</t>
+  </si>
+  <si>
+    <t>004704060033222</t>
+  </si>
+  <si>
+    <t>8866 6566 66666</t>
+  </si>
+  <si>
+    <t>004704060086084</t>
+  </si>
+  <si>
+    <t xml:space="preserve">002704060114851 </t>
+  </si>
+  <si>
+    <t>1220205223980</t>
+  </si>
+  <si>
+    <t>025704061527818</t>
+  </si>
+  <si>
+    <t>0301001441979</t>
+  </si>
+  <si>
+    <t>019704060169767</t>
+  </si>
+  <si>
+    <t>Ngân hàng Techcombank, chi nhánh Đông Đô</t>
+  </si>
+  <si>
+    <t>Ngân hàng Techcombank, chi nhánh Hà Tây - Hà Nội</t>
+  </si>
+  <si>
+    <t>ngân hàng Quốc tế (VIB), chi nhánh Nguyễn Huệ</t>
+  </si>
+  <si>
+    <t>Ngân hàng Techcombank, chi nhánh Hoàng Quốc Việt - Hà Nội</t>
+  </si>
+  <si>
+    <t>Ngân hàng Quốc tế VIB, chi nhánh Hai Bà Trưng - Hà Nội</t>
+  </si>
+  <si>
+    <t>Ngân hàng  thương mại cổ phần quân đội (MB), chi nhánh Điện Biên Phủ</t>
+  </si>
+  <si>
+    <t>Ngân hàng TMCP Quốc Tế Việt Nam (VIB) - Chi nhánh Hai Bà Trưng</t>
+  </si>
+  <si>
+    <t>Ngân hàng Quốc tế VIB, chi nhánh Đống Đa Hà Nội</t>
+  </si>
+  <si>
+    <t>Ngân hàng Agribank, chi nhánh Long Biên</t>
+  </si>
+  <si>
+    <t>Ngân hàng Vietcombank, Chi nhánh Hoàn Kiếm</t>
+  </si>
+  <si>
+    <t>Ngân hàng  Quốc tế VIB, Chi nhánh Hà Đông</t>
+  </si>
+  <si>
+    <t>CT7J, Khu đô thị mới Dương Nội, Hà Đông, Hà Nội</t>
+  </si>
+  <si>
+    <t>Thôn Nghĩa, xã Xuy Xá, Huyện Mỹ Đức, Hà Nội</t>
+  </si>
+  <si>
+    <t>Xóm Cầu, Thanh Liệt, Thanh Trì, TP. Hà Nội</t>
+  </si>
+  <si>
+    <t>P605C, Cư N105, Nguyễn Phong Sắc, Tổ 7, Dịch Vọng Hậu, Cầu Giấy, Hà Nội</t>
+  </si>
+  <si>
+    <t>143 Yên Lãng, Đống Đa, Hà Nội</t>
+  </si>
+  <si>
+    <t>Tổ 4 - Thịnh Liệt - Hoàng Mai - Hà Nội</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2/199 Phú Viên, Tổ 1, Bồ Đề, Long Biên, Hà Nội </t>
+  </si>
+  <si>
+    <t>Cẩm nhượng, Cẩm xuyên, Hà tĩnh</t>
+  </si>
+  <si>
+    <t>Trung Văn - Nam Từ Liêm - Hà Nội</t>
+  </si>
+  <si>
+    <t>Thôn 3, Phúc Hoà, Phúc Thọ, Hà Nội</t>
+  </si>
+  <si>
+    <t>019186009341</t>
+  </si>
+  <si>
+    <t>8019373151</t>
+  </si>
+  <si>
+    <t>8101391805</t>
+  </si>
+  <si>
+    <t>0103417878</t>
+  </si>
+  <si>
+    <t>0103413841</t>
+  </si>
+  <si>
+    <t>8327096826</t>
+  </si>
+  <si>
+    <t>8026501206</t>
+  </si>
+  <si>
+    <t>8009385976</t>
+  </si>
+  <si>
+    <t>8012846722</t>
+  </si>
+  <si>
+    <t>8009473608</t>
+  </si>
+  <si>
+    <t>8539460058</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,6 +588,24 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -816,7 +1014,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
@@ -838,6 +1036,16 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="42" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="10" xfId="42" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="10" xfId="42" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1160,15 +1368,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.81640625" customWidth="1"/>
+    <col min="2" max="2" width="28.08984375" customWidth="1"/>
     <col min="4" max="4" width="23.54296875" customWidth="1"/>
     <col min="5" max="5" width="17.6328125" customWidth="1"/>
     <col min="6" max="6" width="14.90625" customWidth="1"/>
@@ -1178,7 +1386,9 @@
     <col min="11" max="11" width="16.6328125" customWidth="1"/>
     <col min="12" max="12" width="44.453125" customWidth="1"/>
     <col min="13" max="13" width="18.1796875" customWidth="1"/>
-    <col min="16" max="16" width="15" customWidth="1"/>
+    <col min="14" max="14" width="31.81640625" customWidth="1"/>
+    <col min="15" max="15" width="60.26953125" customWidth="1"/>
+    <col min="16" max="16" width="35.6328125" customWidth="1"/>
     <col min="17" max="17" width="14.08984375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14.453125" customWidth="1"/>
   </cols>
@@ -1188,423 +1398,806 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="S1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="T1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="32" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="4"/>
+      <c r="B2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="10">
-        <v>3</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="M2" s="6">
-        <v>41795</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5">
-        <v>12210001259627</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="J2" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="P2" s="19">
+        <v>8077026742</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="S2" s="8"/>
       <c r="T2" s="8"/>
     </row>
-    <row r="3" spans="1:20" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4">
-        <v>3</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="5" t="s">
+    <row r="3" spans="1:20" ht="33.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="4"/>
+      <c r="B3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="5" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="N3" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="J3" s="5">
-        <v>5</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="S3" s="7" t="s">
-        <v>33</v>
-      </c>
+      <c r="O3" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="P3" s="19">
+        <v>8002259299</v>
+      </c>
+      <c r="Q3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="R3" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="S3" s="7"/>
       <c r="T3" s="7"/>
     </row>
-    <row r="4" spans="1:20" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="J4" s="5">
-        <v>3</v>
-      </c>
-      <c r="K4" s="5" t="s">
+    <row r="4" spans="1:20" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="4"/>
+      <c r="B4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="5">
-        <v>1086007000</v>
-      </c>
-      <c r="M4" s="6">
-        <v>43866</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5">
-        <v>50113714007</v>
-      </c>
-      <c r="R4" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="S4" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="C4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="P4" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="R4" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="S4" s="8"/>
       <c r="T4" s="8"/>
     </row>
-    <row r="5" spans="1:20" ht="38.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="5" t="s">
+    <row r="5" spans="1:20" ht="38.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="4"/>
+      <c r="B5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="6">
-        <v>23744</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="J5" s="5">
-        <v>5</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L5" s="10">
-        <v>1065013818</v>
-      </c>
-      <c r="M5" s="6">
-        <v>44474</v>
-      </c>
-      <c r="N5" s="5" t="s">
+      <c r="D5" s="6"/>
+      <c r="E5" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="O5" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="P5" s="5">
-        <v>8111459650</v>
-      </c>
-      <c r="Q5" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="R5" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="S5" s="7" t="s">
-        <v>33</v>
-      </c>
+      <c r="F5" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="K5" s="5"/>
+      <c r="L5" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="P5" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q5" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="S5" s="7"/>
       <c r="T5" s="7"/>
     </row>
-    <row r="6" spans="1:20" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4">
-        <v>2</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="6" t="s">
+    <row r="6" spans="1:20" ht="32.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="4"/>
+      <c r="B6" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="K6" s="5"/>
+      <c r="L6" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="J6" s="5">
-        <v>3</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="M6" s="6">
-        <v>44199</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="R6" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="S6" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="M6" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="P6" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q6" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="R6" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="S6" s="8"/>
       <c r="T6" s="8"/>
     </row>
-    <row r="7" spans="1:20" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4">
-        <v>3</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="5" t="s">
+    <row r="7" spans="1:20" ht="42.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="4"/>
+      <c r="B7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="5"/>
+      <c r="E7" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="K7" s="5"/>
+      <c r="L7" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="M7" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="N7" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="P7" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q7" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="R7" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+    </row>
+    <row r="8" spans="1:20" ht="32" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="4"/>
+      <c r="B8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="K8" s="5"/>
+      <c r="L8" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="M8" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O8" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="P8" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q8" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="R8" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+    </row>
+    <row r="9" spans="1:20" ht="33.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="4"/>
+      <c r="B9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="K9" s="5"/>
+      <c r="L9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O9" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="P9" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q9" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="R9" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+    </row>
+    <row r="10" spans="1:20" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="4"/>
+      <c r="B10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="K10" s="5"/>
+      <c r="L10" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="5" t="s">
+      <c r="M10" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O10" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="P10" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q10" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="R10" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+    </row>
+    <row r="11" spans="1:20" ht="38.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="4"/>
+      <c r="B11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="K11" s="5"/>
+      <c r="L11" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I7" s="5" t="s">
+      <c r="M11" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="J7" s="5">
-        <v>5</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="O7" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="P7" s="5">
-        <v>8129082973</v>
-      </c>
-      <c r="Q7" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="R7" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="S7" s="7" t="s">
+      <c r="N11" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O11" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="P11" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q11" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="R11" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+    </row>
+    <row r="12" spans="1:20" ht="32.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="4"/>
+      <c r="B12" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="T7" s="7"/>
+      <c r="C12" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="K12" s="5"/>
+      <c r="L12" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="M12" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="N12" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O12" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="P12" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q12" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="R12" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+    </row>
+    <row r="13" spans="1:20" ht="42.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="4"/>
+      <c r="B13" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="K13" s="5"/>
+      <c r="L13" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="M13" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="N13" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O13" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="P13" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q13" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="R13" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+    </row>
+    <row r="14" spans="1:20" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+    </row>
+    <row r="15" spans="1:20" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+    </row>
+    <row r="16" spans="1:20" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+    </row>
+    <row r="17" spans="1:20" ht="38.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+    </row>
+    <row r="18" spans="1:20" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="8"/>
+      <c r="T18" s="8"/>
+    </row>
+    <row r="19" spans="1:20" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1"/>
     <hyperlink ref="F2" r:id="rId2"/>
-    <hyperlink ref="F5" r:id="rId3"/>
-    <hyperlink ref="F4" r:id="rId4"/>
-    <hyperlink ref="F7" r:id="rId5"/>
-    <hyperlink ref="F6" r:id="rId6"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F6" r:id="rId4"/>
+    <hyperlink ref="F5" r:id="rId5"/>
+    <hyperlink ref="F7" r:id="rId6"/>
+    <hyperlink ref="F8" r:id="rId7"/>
+    <hyperlink ref="F12" r:id="rId8"/>
+    <hyperlink ref="F13" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix exportHopDong và cập nhật học vị
</commit_message>
<xml_diff>
--- a/uploads/Điền thông tin GV mời KTMT 29102024(Sheet1)1 - Copy.xlsx
+++ b/uploads/Điền thông tin GV mời KTMT 29102024(Sheet1)1 - Copy.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="127">
   <si>
     <t>STT</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Nam</t>
   </si>
   <si>
-    <t>Khá</t>
-  </si>
-  <si>
     <t>Họ và tên</t>
   </si>
   <si>
@@ -90,173 +87,326 @@
     <t>Giảng viên</t>
   </si>
   <si>
-    <t>CCSĐKQLCTVDLQGVDC</t>
-  </si>
-  <si>
     <t>Thạc sĩ</t>
   </si>
   <si>
-    <t>Học viện Tài chính</t>
-  </si>
-  <si>
-    <t>Công ty TNHH phần mềm FPT</t>
-  </si>
-  <si>
-    <t>21/12/1980</t>
-  </si>
-  <si>
-    <t>chungphamdinh@gmail.com</t>
-  </si>
-  <si>
-    <t>Phạm Đình Chung</t>
-  </si>
-  <si>
-    <t>CA TP Hà Nội</t>
-  </si>
-  <si>
-    <t>14/80 Lê Trọng Tấn, Thanh Xuân, Hà Nội</t>
-  </si>
-  <si>
-    <t>Ngân hàng BIDV, chi nhánh Hà Thành, Hà Nội</t>
-  </si>
-  <si>
-    <t>DTVT</t>
-  </si>
-  <si>
-    <t>Nguyễn Thế Truyện</t>
-  </si>
-  <si>
-    <t>23/4/1964</t>
-  </si>
-  <si>
-    <t>truyennt6868@gmail.com</t>
-  </si>
-  <si>
-    <t>Viện trưởng</t>
-  </si>
-  <si>
-    <t>29/2/2016</t>
-  </si>
-  <si>
-    <t>Trần Anh Dũng</t>
-  </si>
-  <si>
-    <t>Đinh Văn Tuân</t>
-  </si>
-  <si>
-    <t>Đinh Nho Thanh</t>
-  </si>
-  <si>
-    <t>Đặng Trần Chuyên</t>
-  </si>
-  <si>
-    <t>21/06/1986</t>
-  </si>
-  <si>
-    <t>18/9/1957</t>
-  </si>
-  <si>
-    <t>23/4/1966</t>
-  </si>
-  <si>
-    <t>0989290754</t>
-  </si>
-  <si>
-    <t>0912095442</t>
-  </si>
-  <si>
-    <t>0984210686</t>
-  </si>
-  <si>
-    <t>0947365469</t>
-  </si>
-  <si>
-    <t>0389363125</t>
-  </si>
-  <si>
-    <t>0903433199</t>
-  </si>
-  <si>
-    <t>trananhdung21@gmail.com</t>
-  </si>
-  <si>
-    <t>Tiến sĩ</t>
-  </si>
-  <si>
-    <t>Giám đốc</t>
-  </si>
-  <si>
-    <t>Phó giám đốc</t>
-  </si>
-  <si>
-    <t>Nghỉ hưu</t>
-  </si>
-  <si>
-    <t>026080000033</t>
-  </si>
-  <si>
-    <t>027064000071</t>
-  </si>
-  <si>
-    <t>031057006770</t>
-  </si>
-  <si>
-    <t>001066011844</t>
-  </si>
-  <si>
-    <t>15/3/2018</t>
-  </si>
-  <si>
-    <t>Cục Cảnh Sát ĐKQL Cư trú và DLQG về Dân cư</t>
-  </si>
-  <si>
-    <t>0011000453665</t>
-  </si>
-  <si>
-    <t>22010000744116</t>
-  </si>
-  <si>
-    <t>0020149984004</t>
-  </si>
-  <si>
-    <t>11521988293018</t>
-  </si>
-  <si>
-    <t>Ngân hàng Techcombank, chi nhánh Ngọc Khánh, Hà Nội.</t>
-  </si>
-  <si>
-    <t>Ngân hàng Quân đội, chi nhánh hội sở chính</t>
-  </si>
-  <si>
-    <t>Ngân hàng BIDV</t>
-  </si>
-  <si>
-    <t>Ngân hàng quân đội MB. Chi nhánh MB Trần Duy Hưng</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ngân hàng TMCP Ngoại thương </t>
-  </si>
-  <si>
-    <t>Số 25 ngõ 42 Trần Cung, Cổ Nhuế, Bắc Từ Liêm, Hà Nội</t>
-  </si>
-  <si>
-    <t>P410, A12, Kim Giang - Thanh Xuân - Hà Nội</t>
-  </si>
-  <si>
-    <t>P 2707 Tòa E Tòa nhà  Mulberry Lane, Mộ  Lao, Hà Đông, Hà Nội</t>
-  </si>
-  <si>
-    <t>P1122 HH1C Linh Đàm, Hoàng Liệt, Hoàng Mai, Hà Nội</t>
-  </si>
-  <si>
-    <t>Căn A2102 Chung cư Hồng Kong, 243A Đê La Thành, Phường Láng Thượng, Quận Đống Đa Hà Nội</t>
+    <t>Nguyễn Thị Thanh Tâm</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Tới</t>
+  </si>
+  <si>
+    <t>Đặng Thị Kim Anh</t>
+  </si>
+  <si>
+    <t>Bùi Văn Công</t>
+  </si>
+  <si>
+    <t>Bùi Thị Như</t>
+  </si>
+  <si>
+    <t>Trịnh Anh Tuấn</t>
+  </si>
+  <si>
+    <t>Đỗ Bảo Sơn</t>
+  </si>
+  <si>
+    <t>Lê Thanh Tấn</t>
+  </si>
+  <si>
+    <t>Nguyễn Hưng Long</t>
+  </si>
+  <si>
+    <t>Nguyễn Thái Sơn</t>
+  </si>
+  <si>
+    <t>Trịnh Thị Xuân</t>
+  </si>
+  <si>
+    <t>Khuất Thị Ngọc Ánh</t>
+  </si>
+  <si>
+    <t>Nữ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04/08/2022        </t>
+  </si>
+  <si>
+    <t>Cục QLHC về trật tự xã hội</t>
+  </si>
+  <si>
+    <t>024079016540</t>
+  </si>
+  <si>
+    <t>04/08/2022</t>
+  </si>
+  <si>
+    <t>001182007087</t>
+  </si>
+  <si>
+    <t>07/04/2015</t>
+  </si>
+  <si>
+    <t>036083007024</t>
+  </si>
+  <si>
+    <t>30/04/2021</t>
+  </si>
+  <si>
+    <t>034185001956</t>
+  </si>
+  <si>
+    <t>02/08/2022</t>
+  </si>
+  <si>
+    <t>034083012886</t>
+  </si>
+  <si>
+    <t>031091011464</t>
+  </si>
+  <si>
+    <t>02/06/2020</t>
+  </si>
+  <si>
+    <t>030079009486</t>
+  </si>
+  <si>
+    <t>29/03/2021</t>
+  </si>
+  <si>
+    <t>001069003204</t>
+  </si>
+  <si>
+    <t>24/6/2021</t>
+  </si>
+  <si>
+    <t>042081016692</t>
+  </si>
+  <si>
+    <t>08/01/2022</t>
+  </si>
+  <si>
+    <t>038179013948</t>
+  </si>
+  <si>
+    <t>07/04/2021</t>
+  </si>
+  <si>
+    <t>001196016484</t>
+  </si>
+  <si>
+    <t>14/06/2022</t>
+  </si>
+  <si>
+    <t>0973002640</t>
+  </si>
+  <si>
+    <t>0867536913</t>
+  </si>
+  <si>
+    <t>0904876082</t>
+  </si>
+  <si>
+    <t>0983978015</t>
+  </si>
+  <si>
+    <t>0936507189</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0919200290 </t>
+  </si>
+  <si>
+    <t>0332336863</t>
+  </si>
+  <si>
+    <t>0912345399</t>
+  </si>
+  <si>
+    <t>0979734899</t>
+  </si>
+  <si>
+    <t>0969880912</t>
+  </si>
+  <si>
+    <t>0982083232</t>
+  </si>
+  <si>
+    <t>0392120967</t>
+  </si>
+  <si>
+    <t>ttvancntt@gmai.com</t>
+  </si>
+  <si>
+    <t>kimanh0602@gmail.com</t>
+  </si>
+  <si>
+    <t>bvcoong@gmail.com</t>
+  </si>
+  <si>
+    <t>nhubt1983@gmail.com</t>
+  </si>
+  <si>
+    <t>txtuan@gmail.com</t>
+  </si>
+  <si>
+    <t>sondb19@gmail.com</t>
+  </si>
+  <si>
+    <t>thanhtanhd@gmail.com</t>
+  </si>
+  <si>
+    <t>longtmu@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> thaison.nguyenn@gmail.com</t>
+  </si>
+  <si>
+    <t>trinhxuan@gmail.com</t>
+  </si>
+  <si>
+    <t>anhktn@utt.edu.vn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiến sỹ    </t>
+  </si>
+  <si>
+    <t>Nghiên cứu viên</t>
+  </si>
+  <si>
+    <t>Giảng viên chính</t>
+  </si>
+  <si>
+    <t>3.85</t>
+  </si>
+  <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>3.99</t>
+  </si>
+  <si>
+    <t>3.66</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>6.1</t>
+  </si>
+  <si>
+    <t>2.67</t>
+  </si>
+  <si>
+    <t>19036428472018</t>
+  </si>
+  <si>
+    <t>19033849649015</t>
+  </si>
+  <si>
+    <t>019704060203270</t>
+  </si>
+  <si>
+    <t>11121651434010</t>
+  </si>
+  <si>
+    <t>004704060033222</t>
+  </si>
+  <si>
+    <t>8866 6566 66666</t>
+  </si>
+  <si>
+    <t>004704060086084</t>
+  </si>
+  <si>
+    <t xml:space="preserve">002704060114851 </t>
+  </si>
+  <si>
+    <t>1220205223980</t>
+  </si>
+  <si>
+    <t>025704061527818</t>
+  </si>
+  <si>
+    <t>0301001441979</t>
+  </si>
+  <si>
+    <t>019704060169767</t>
+  </si>
+  <si>
+    <t>Ngân hàng Techcombank, chi nhánh Đông Đô</t>
+  </si>
+  <si>
+    <t>Ngân hàng Techcombank, chi nhánh Hà Tây - Hà Nội</t>
+  </si>
+  <si>
+    <t>ngân hàng Quốc tế (VIB), chi nhánh Nguyễn Huệ</t>
+  </si>
+  <si>
+    <t>Ngân hàng Techcombank, chi nhánh Hoàng Quốc Việt - Hà Nội</t>
+  </si>
+  <si>
+    <t>Ngân hàng Quốc tế VIB, chi nhánh Hai Bà Trưng - Hà Nội</t>
+  </si>
+  <si>
+    <t>Ngân hàng  thương mại cổ phần quân đội (MB), chi nhánh Điện Biên Phủ</t>
+  </si>
+  <si>
+    <t>Ngân hàng TMCP Quốc Tế Việt Nam (VIB) - Chi nhánh Hai Bà Trưng</t>
+  </si>
+  <si>
+    <t>Ngân hàng Quốc tế VIB, chi nhánh Đống Đa Hà Nội</t>
+  </si>
+  <si>
+    <t>Ngân hàng Agribank, chi nhánh Long Biên</t>
+  </si>
+  <si>
+    <t>Ngân hàng Vietcombank, Chi nhánh Hoàn Kiếm</t>
+  </si>
+  <si>
+    <t>Ngân hàng  Quốc tế VIB, Chi nhánh Hà Đông</t>
+  </si>
+  <si>
+    <t>CT7J, Khu đô thị mới Dương Nội, Hà Đông, Hà Nội</t>
+  </si>
+  <si>
+    <t>Thôn Nghĩa, xã Xuy Xá, Huyện Mỹ Đức, Hà Nội</t>
+  </si>
+  <si>
+    <t>Xóm Cầu, Thanh Liệt, Thanh Trì, TP. Hà Nội</t>
+  </si>
+  <si>
+    <t>P605C, Cư N105, Nguyễn Phong Sắc, Tổ 7, Dịch Vọng Hậu, Cầu Giấy, Hà Nội</t>
+  </si>
+  <si>
+    <t>143 Yên Lãng, Đống Đa, Hà Nội</t>
+  </si>
+  <si>
+    <t>Tổ 4 - Thịnh Liệt - Hoàng Mai - Hà Nội</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2/199 Phú Viên, Tổ 1, Bồ Đề, Long Biên, Hà Nội </t>
+  </si>
+  <si>
+    <t>Cẩm nhượng, Cẩm xuyên, Hà tĩnh</t>
+  </si>
+  <si>
+    <t>Trung Văn - Nam Từ Liêm - Hà Nội</t>
+  </si>
+  <si>
+    <t>Thôn 3, Phúc Hoà, Phúc Thọ, Hà Nội</t>
+  </si>
+  <si>
+    <t>019186009341</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,6 +558,24 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -816,7 +984,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
@@ -838,6 +1006,16 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="42" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="10" xfId="42" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="10" xfId="42" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1160,15 +1338,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.81640625" customWidth="1"/>
+    <col min="2" max="2" width="28.08984375" customWidth="1"/>
     <col min="4" max="4" width="23.54296875" customWidth="1"/>
     <col min="5" max="5" width="17.6328125" customWidth="1"/>
     <col min="6" max="6" width="14.90625" customWidth="1"/>
@@ -1178,6 +1356,8 @@
     <col min="11" max="11" width="16.6328125" customWidth="1"/>
     <col min="12" max="12" width="44.453125" customWidth="1"/>
     <col min="13" max="13" width="18.1796875" customWidth="1"/>
+    <col min="14" max="14" width="31.81640625" customWidth="1"/>
+    <col min="15" max="15" width="42.6328125" customWidth="1"/>
     <col min="16" max="16" width="15" customWidth="1"/>
     <col min="17" max="17" width="14.08984375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14.453125" customWidth="1"/>
@@ -1188,423 +1368,782 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="S1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="T1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="32" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="4"/>
+      <c r="B2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="10">
-        <v>3</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="M2" s="6">
-        <v>41795</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>31</v>
+      <c r="J2" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>116</v>
       </c>
       <c r="P2" s="5"/>
-      <c r="Q2" s="5">
-        <v>12210001259627</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="Q2" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="S2" s="8"/>
       <c r="T2" s="8"/>
     </row>
-    <row r="3" spans="1:20" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4">
-        <v>3</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="5" t="s">
+    <row r="3" spans="1:20" ht="33.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="4"/>
+      <c r="B3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="5" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="N3" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="J3" s="5">
-        <v>5</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>72</v>
+      <c r="O3" s="11" t="s">
+        <v>116</v>
       </c>
       <c r="P3" s="5"/>
-      <c r="Q3" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="S3" s="7" t="s">
-        <v>33</v>
-      </c>
+      <c r="Q3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="R3" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="S3" s="7"/>
       <c r="T3" s="7"/>
     </row>
-    <row r="4" spans="1:20" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="J4" s="5">
-        <v>3</v>
-      </c>
-      <c r="K4" s="5" t="s">
+    <row r="4" spans="1:20" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="4"/>
+      <c r="B4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="5">
-        <v>1086007000</v>
-      </c>
-      <c r="M4" s="6">
-        <v>43866</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>73</v>
+      <c r="C4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>117</v>
       </c>
       <c r="P4" s="5"/>
-      <c r="Q4" s="5">
-        <v>50113714007</v>
-      </c>
-      <c r="R4" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="S4" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="Q4" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="R4" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="S4" s="8"/>
       <c r="T4" s="8"/>
     </row>
-    <row r="5" spans="1:20" ht="38.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="5" t="s">
+    <row r="5" spans="1:20" ht="38.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="4"/>
+      <c r="B5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="6">
-        <v>23744</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="J5" s="5">
-        <v>5</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L5" s="10">
-        <v>1065013818</v>
-      </c>
-      <c r="M5" s="6">
-        <v>44474</v>
-      </c>
-      <c r="N5" s="5" t="s">
+      <c r="D5" s="6"/>
+      <c r="E5" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="O5" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="P5" s="5">
-        <v>8111459650</v>
-      </c>
-      <c r="Q5" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="R5" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="S5" s="7" t="s">
-        <v>33</v>
-      </c>
+      <c r="F5" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="K5" s="5"/>
+      <c r="L5" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="S5" s="7"/>
       <c r="T5" s="7"/>
     </row>
-    <row r="6" spans="1:20" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4">
-        <v>2</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="6" t="s">
+    <row r="6" spans="1:20" ht="32.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="4"/>
+      <c r="B6" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="K6" s="5"/>
+      <c r="L6" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="J6" s="5">
-        <v>3</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="M6" s="6">
-        <v>44199</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>75</v>
+      <c r="M6" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>119</v>
       </c>
       <c r="P6" s="5"/>
-      <c r="Q6" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="R6" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="S6" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="Q6" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="R6" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="S6" s="8"/>
       <c r="T6" s="8"/>
     </row>
-    <row r="7" spans="1:20" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4">
-        <v>3</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="5" t="s">
+    <row r="7" spans="1:20" ht="42.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="4"/>
+      <c r="B7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="5"/>
+      <c r="E7" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="K7" s="5"/>
+      <c r="L7" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="M7" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="N7" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="R7" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+    </row>
+    <row r="8" spans="1:20" ht="32" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="4"/>
+      <c r="B8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="K8" s="5"/>
+      <c r="L8" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="M8" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O8" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="R8" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+    </row>
+    <row r="9" spans="1:20" ht="33.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="4"/>
+      <c r="B9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="K9" s="5"/>
+      <c r="L9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O9" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="R9" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+    </row>
+    <row r="10" spans="1:20" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="4"/>
+      <c r="B10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="K10" s="5"/>
+      <c r="L10" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="5" t="s">
+      <c r="M10" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O10" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="R10" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+    </row>
+    <row r="11" spans="1:20" ht="38.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="4"/>
+      <c r="B11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="K11" s="5"/>
+      <c r="L11" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I7" s="5" t="s">
+      <c r="M11" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="J7" s="5">
-        <v>5</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="O7" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="P7" s="5">
-        <v>8129082973</v>
-      </c>
-      <c r="Q7" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="R7" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="S7" s="7" t="s">
+      <c r="N11" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O11" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="R11" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+    </row>
+    <row r="12" spans="1:20" ht="32.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="4"/>
+      <c r="B12" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="T7" s="7"/>
+      <c r="C12" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="K12" s="5"/>
+      <c r="L12" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="M12" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="N12" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O12" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="R12" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+    </row>
+    <row r="13" spans="1:20" ht="42.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="4"/>
+      <c r="B13" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="K13" s="5"/>
+      <c r="L13" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="M13" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="N13" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O13" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="R13" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+    </row>
+    <row r="14" spans="1:20" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+    </row>
+    <row r="15" spans="1:20" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+    </row>
+    <row r="16" spans="1:20" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+    </row>
+    <row r="17" spans="1:20" ht="38.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+    </row>
+    <row r="18" spans="1:20" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="8"/>
+      <c r="T18" s="8"/>
+    </row>
+    <row r="19" spans="1:20" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1"/>
     <hyperlink ref="F2" r:id="rId2"/>
-    <hyperlink ref="F5" r:id="rId3"/>
-    <hyperlink ref="F4" r:id="rId4"/>
-    <hyperlink ref="F7" r:id="rId5"/>
-    <hyperlink ref="F6" r:id="rId6"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F6" r:id="rId4"/>
+    <hyperlink ref="F5" r:id="rId5"/>
+    <hyperlink ref="F7" r:id="rId6"/>
+    <hyperlink ref="F8" r:id="rId7"/>
+    <hyperlink ref="F12" r:id="rId8"/>
+    <hyperlink ref="F13" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix importGvmList: chỉ không chèn những giảng viên trùng CCCD
</commit_message>
<xml_diff>
--- a/uploads/Điền thông tin GV mời KTMT 29102024(Sheet1)1 - Copy.xlsx
+++ b/uploads/Điền thông tin GV mời KTMT 29102024(Sheet1)1 - Copy.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="137">
   <si>
     <t>STT</t>
   </si>
@@ -400,6 +400,36 @@
   </si>
   <si>
     <t>019186009341</t>
+  </si>
+  <si>
+    <t>8019373151</t>
+  </si>
+  <si>
+    <t>8101391805</t>
+  </si>
+  <si>
+    <t>0103417878</t>
+  </si>
+  <si>
+    <t>0103413841</t>
+  </si>
+  <si>
+    <t>8327096826</t>
+  </si>
+  <si>
+    <t>8026501206</t>
+  </si>
+  <si>
+    <t>8009385976</t>
+  </si>
+  <si>
+    <t>8012846722</t>
+  </si>
+  <si>
+    <t>8009473608</t>
+  </si>
+  <si>
+    <t>8539460058</t>
   </si>
 </sst>
 </file>
@@ -1340,8 +1370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1357,10 +1387,10 @@
     <col min="12" max="12" width="44.453125" customWidth="1"/>
     <col min="13" max="13" width="18.1796875" customWidth="1"/>
     <col min="14" max="14" width="31.81640625" customWidth="1"/>
-    <col min="15" max="15" width="42.6328125" customWidth="1"/>
-    <col min="16" max="16" width="15" customWidth="1"/>
+    <col min="15" max="15" width="60.26953125" customWidth="1"/>
+    <col min="16" max="16" width="35.6328125" customWidth="1"/>
     <col min="17" max="17" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.453125" customWidth="1"/>
+    <col min="18" max="18" width="81.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="16.5" x14ac:dyDescent="0.35">
@@ -1463,7 +1493,9 @@
       <c r="O2" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="P2" s="5"/>
+      <c r="P2" s="19">
+        <v>8077026742</v>
+      </c>
       <c r="Q2" s="12" t="s">
         <v>93</v>
       </c>
@@ -1511,7 +1543,9 @@
       <c r="O3" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="P3" s="5"/>
+      <c r="P3" s="19">
+        <v>8002259299</v>
+      </c>
       <c r="Q3" s="12" t="s">
         <v>94</v>
       </c>
@@ -1559,7 +1593,9 @@
       <c r="O4" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="P4" s="5"/>
+      <c r="P4" s="13" t="s">
+        <v>127</v>
+      </c>
       <c r="Q4" s="13" t="s">
         <v>95</v>
       </c>
@@ -1607,7 +1643,9 @@
       <c r="O5" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="P5" s="5"/>
+      <c r="P5" s="12" t="s">
+        <v>128</v>
+      </c>
       <c r="Q5" s="12" t="s">
         <v>96</v>
       </c>
@@ -1655,7 +1693,9 @@
       <c r="O6" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="P6" s="5"/>
+      <c r="P6" s="13" t="s">
+        <v>129</v>
+      </c>
       <c r="Q6" s="13" t="s">
         <v>97</v>
       </c>
@@ -1703,7 +1743,9 @@
       <c r="O7" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="P7" s="5"/>
+      <c r="P7" s="13" t="s">
+        <v>130</v>
+      </c>
       <c r="Q7" s="13" t="s">
         <v>98</v>
       </c>
@@ -1751,7 +1793,9 @@
       <c r="O8" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="P8" s="5"/>
+      <c r="P8" s="13" t="s">
+        <v>131</v>
+      </c>
       <c r="Q8" s="13" t="s">
         <v>99</v>
       </c>
@@ -1799,7 +1843,9 @@
       <c r="O9" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="P9" s="5"/>
+      <c r="P9" s="13" t="s">
+        <v>132</v>
+      </c>
       <c r="Q9" s="13" t="s">
         <v>100</v>
       </c>
@@ -1847,7 +1893,9 @@
       <c r="O10" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="P10" s="5"/>
+      <c r="P10" s="13" t="s">
+        <v>133</v>
+      </c>
       <c r="Q10" s="13" t="s">
         <v>101</v>
       </c>
@@ -1895,7 +1943,9 @@
       <c r="O11" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="P11" s="5"/>
+      <c r="P11" s="13" t="s">
+        <v>134</v>
+      </c>
       <c r="Q11" s="13" t="s">
         <v>102</v>
       </c>
@@ -1943,7 +1993,9 @@
       <c r="O12" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="P12" s="5"/>
+      <c r="P12" s="13" t="s">
+        <v>135</v>
+      </c>
       <c r="Q12" s="13" t="s">
         <v>103</v>
       </c>
@@ -1991,7 +2043,9 @@
       <c r="O13" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="P13" s="5"/>
+      <c r="P13" s="13" t="s">
+        <v>136</v>
+      </c>
       <c r="Q13" s="13" t="s">
         <v>104</v>
       </c>

</xml_diff>

<commit_message>
thêm (A) nếu trùng tên bên importGvmList
</commit_message>
<xml_diff>
--- a/uploads/Điền thông tin GV mời KTMT 29102024(Sheet1)1 - Copy.xlsx
+++ b/uploads/Điền thông tin GV mời KTMT 29102024(Sheet1)1 - Copy.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_ttcs\uploadWithCoundinary\dữ liệu demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_ttcs\uploadWithCoundinary\dữ liệu demo\tet trùng tên\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="138">
   <si>
     <t>STT</t>
   </si>
@@ -135,15 +135,9 @@
     <t>Cục QLHC về trật tự xã hội</t>
   </si>
   <si>
-    <t>024079016540</t>
-  </si>
-  <si>
     <t>04/08/2022</t>
   </si>
   <si>
-    <t>001182007087</t>
-  </si>
-  <si>
     <t>07/04/2015</t>
   </si>
   <si>
@@ -201,235 +195,244 @@
     <t>0973002640</t>
   </si>
   <si>
+    <t>0983978015</t>
+  </si>
+  <si>
+    <t>0936507189</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0919200290 </t>
+  </si>
+  <si>
+    <t>0332336863</t>
+  </si>
+  <si>
+    <t>0912345399</t>
+  </si>
+  <si>
+    <t>0979734899</t>
+  </si>
+  <si>
+    <t>0969880912</t>
+  </si>
+  <si>
+    <t>0982083232</t>
+  </si>
+  <si>
+    <t>0392120967</t>
+  </si>
+  <si>
+    <t>ttvancntt@gmai.com</t>
+  </si>
+  <si>
+    <t>kimanh0602@gmail.com</t>
+  </si>
+  <si>
+    <t>bvcoong@gmail.com</t>
+  </si>
+  <si>
+    <t>nhubt1983@gmail.com</t>
+  </si>
+  <si>
+    <t>txtuan@gmail.com</t>
+  </si>
+  <si>
+    <t>sondb19@gmail.com</t>
+  </si>
+  <si>
+    <t>thanhtanhd@gmail.com</t>
+  </si>
+  <si>
+    <t>longtmu@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> thaison.nguyenn@gmail.com</t>
+  </si>
+  <si>
+    <t>trinhxuan@gmail.com</t>
+  </si>
+  <si>
+    <t>anhktn@utt.edu.vn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiến sỹ    </t>
+  </si>
+  <si>
+    <t>Nghiên cứu viên</t>
+  </si>
+  <si>
+    <t>Giảng viên chính</t>
+  </si>
+  <si>
+    <t>3.85</t>
+  </si>
+  <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>3.99</t>
+  </si>
+  <si>
+    <t>3.66</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>6.1</t>
+  </si>
+  <si>
+    <t>2.67</t>
+  </si>
+  <si>
+    <t>19036428472018</t>
+  </si>
+  <si>
+    <t>19033849649015</t>
+  </si>
+  <si>
+    <t>019704060203270</t>
+  </si>
+  <si>
+    <t>11121651434010</t>
+  </si>
+  <si>
+    <t>004704060033222</t>
+  </si>
+  <si>
+    <t>8866 6566 66666</t>
+  </si>
+  <si>
+    <t>004704060086084</t>
+  </si>
+  <si>
+    <t xml:space="preserve">002704060114851 </t>
+  </si>
+  <si>
+    <t>1220205223980</t>
+  </si>
+  <si>
+    <t>025704061527818</t>
+  </si>
+  <si>
+    <t>0301001441979</t>
+  </si>
+  <si>
+    <t>019704060169767</t>
+  </si>
+  <si>
+    <t>Ngân hàng Techcombank, chi nhánh Đông Đô</t>
+  </si>
+  <si>
+    <t>Ngân hàng Techcombank, chi nhánh Hà Tây - Hà Nội</t>
+  </si>
+  <si>
+    <t>ngân hàng Quốc tế (VIB), chi nhánh Nguyễn Huệ</t>
+  </si>
+  <si>
+    <t>Ngân hàng Techcombank, chi nhánh Hoàng Quốc Việt - Hà Nội</t>
+  </si>
+  <si>
+    <t>Ngân hàng Quốc tế VIB, chi nhánh Hai Bà Trưng - Hà Nội</t>
+  </si>
+  <si>
+    <t>Ngân hàng  thương mại cổ phần quân đội (MB), chi nhánh Điện Biên Phủ</t>
+  </si>
+  <si>
+    <t>Ngân hàng TMCP Quốc Tế Việt Nam (VIB) - Chi nhánh Hai Bà Trưng</t>
+  </si>
+  <si>
+    <t>Ngân hàng Quốc tế VIB, chi nhánh Đống Đa Hà Nội</t>
+  </si>
+  <si>
+    <t>Ngân hàng Agribank, chi nhánh Long Biên</t>
+  </si>
+  <si>
+    <t>Ngân hàng Vietcombank, Chi nhánh Hoàn Kiếm</t>
+  </si>
+  <si>
+    <t>Ngân hàng  Quốc tế VIB, Chi nhánh Hà Đông</t>
+  </si>
+  <si>
+    <t>CT7J, Khu đô thị mới Dương Nội, Hà Đông, Hà Nội</t>
+  </si>
+  <si>
+    <t>Thôn Nghĩa, xã Xuy Xá, Huyện Mỹ Đức, Hà Nội</t>
+  </si>
+  <si>
+    <t>Xóm Cầu, Thanh Liệt, Thanh Trì, TP. Hà Nội</t>
+  </si>
+  <si>
+    <t>P605C, Cư N105, Nguyễn Phong Sắc, Tổ 7, Dịch Vọng Hậu, Cầu Giấy, Hà Nội</t>
+  </si>
+  <si>
+    <t>143 Yên Lãng, Đống Đa, Hà Nội</t>
+  </si>
+  <si>
+    <t>Tổ 4 - Thịnh Liệt - Hoàng Mai - Hà Nội</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2/199 Phú Viên, Tổ 1, Bồ Đề, Long Biên, Hà Nội </t>
+  </si>
+  <si>
+    <t>Cẩm nhượng, Cẩm xuyên, Hà tĩnh</t>
+  </si>
+  <si>
+    <t>Trung Văn - Nam Từ Liêm - Hà Nội</t>
+  </si>
+  <si>
+    <t>Thôn 3, Phúc Hoà, Phúc Thọ, Hà Nội</t>
+  </si>
+  <si>
+    <t>019186009341</t>
+  </si>
+  <si>
+    <t>8019373151</t>
+  </si>
+  <si>
+    <t>8101391805</t>
+  </si>
+  <si>
+    <t>0103417878</t>
+  </si>
+  <si>
+    <t>0103413841</t>
+  </si>
+  <si>
+    <t>8327096826</t>
+  </si>
+  <si>
+    <t>8026501206</t>
+  </si>
+  <si>
+    <t>8009385976</t>
+  </si>
+  <si>
+    <t>8012846722</t>
+  </si>
+  <si>
+    <t>8009473608</t>
+  </si>
+  <si>
+    <t>8539460058</t>
+  </si>
+  <si>
     <t>0867536913</t>
   </si>
   <si>
     <t>0904876082</t>
   </si>
   <si>
-    <t>0983978015</t>
-  </si>
-  <si>
-    <t>0936507189</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0919200290 </t>
-  </si>
-  <si>
-    <t>0332336863</t>
-  </si>
-  <si>
-    <t>0912345399</t>
-  </si>
-  <si>
-    <t>0979734899</t>
-  </si>
-  <si>
-    <t>0969880912</t>
-  </si>
-  <si>
-    <t>0982083232</t>
-  </si>
-  <si>
-    <t>0392120967</t>
-  </si>
-  <si>
-    <t>ttvancntt@gmai.com</t>
-  </si>
-  <si>
-    <t>kimanh0602@gmail.com</t>
-  </si>
-  <si>
-    <t>bvcoong@gmail.com</t>
-  </si>
-  <si>
-    <t>nhubt1983@gmail.com</t>
-  </si>
-  <si>
-    <t>txtuan@gmail.com</t>
-  </si>
-  <si>
-    <t>sondb19@gmail.com</t>
-  </si>
-  <si>
-    <t>thanhtanhd@gmail.com</t>
-  </si>
-  <si>
-    <t>longtmu@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> thaison.nguyenn@gmail.com</t>
-  </si>
-  <si>
-    <t>trinhxuan@gmail.com</t>
-  </si>
-  <si>
-    <t>anhktn@utt.edu.vn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiến sỹ    </t>
-  </si>
-  <si>
-    <t>Nghiên cứu viên</t>
-  </si>
-  <si>
-    <t>Giảng viên chính</t>
-  </si>
-  <si>
-    <t>3.85</t>
-  </si>
-  <si>
-    <t>5.5</t>
-  </si>
-  <si>
-    <t>3.6</t>
-  </si>
-  <si>
-    <t>3.99</t>
-  </si>
-  <si>
-    <t>3.66</t>
-  </si>
-  <si>
-    <t>3.0</t>
-  </si>
-  <si>
-    <t>6.1</t>
-  </si>
-  <si>
-    <t>2.67</t>
-  </si>
-  <si>
-    <t>19036428472018</t>
-  </si>
-  <si>
-    <t>19033849649015</t>
-  </si>
-  <si>
-    <t>019704060203270</t>
-  </si>
-  <si>
-    <t>11121651434010</t>
-  </si>
-  <si>
-    <t>004704060033222</t>
-  </si>
-  <si>
-    <t>8866 6566 66666</t>
-  </si>
-  <si>
-    <t>004704060086084</t>
-  </si>
-  <si>
-    <t xml:space="preserve">002704060114851 </t>
-  </si>
-  <si>
-    <t>1220205223980</t>
-  </si>
-  <si>
-    <t>025704061527818</t>
-  </si>
-  <si>
-    <t>0301001441979</t>
-  </si>
-  <si>
-    <t>019704060169767</t>
-  </si>
-  <si>
-    <t>Ngân hàng Techcombank, chi nhánh Đông Đô</t>
-  </si>
-  <si>
-    <t>Ngân hàng Techcombank, chi nhánh Hà Tây - Hà Nội</t>
-  </si>
-  <si>
-    <t>ngân hàng Quốc tế (VIB), chi nhánh Nguyễn Huệ</t>
-  </si>
-  <si>
-    <t>Ngân hàng Techcombank, chi nhánh Hoàng Quốc Việt - Hà Nội</t>
-  </si>
-  <si>
-    <t>Ngân hàng Quốc tế VIB, chi nhánh Hai Bà Trưng - Hà Nội</t>
-  </si>
-  <si>
-    <t>Ngân hàng  thương mại cổ phần quân đội (MB), chi nhánh Điện Biên Phủ</t>
-  </si>
-  <si>
-    <t>Ngân hàng TMCP Quốc Tế Việt Nam (VIB) - Chi nhánh Hai Bà Trưng</t>
-  </si>
-  <si>
-    <t>Ngân hàng Quốc tế VIB, chi nhánh Đống Đa Hà Nội</t>
-  </si>
-  <si>
-    <t>Ngân hàng Agribank, chi nhánh Long Biên</t>
-  </si>
-  <si>
-    <t>Ngân hàng Vietcombank, Chi nhánh Hoàn Kiếm</t>
-  </si>
-  <si>
-    <t>Ngân hàng  Quốc tế VIB, Chi nhánh Hà Đông</t>
-  </si>
-  <si>
-    <t>CT7J, Khu đô thị mới Dương Nội, Hà Đông, Hà Nội</t>
-  </si>
-  <si>
-    <t>Thôn Nghĩa, xã Xuy Xá, Huyện Mỹ Đức, Hà Nội</t>
-  </si>
-  <si>
-    <t>Xóm Cầu, Thanh Liệt, Thanh Trì, TP. Hà Nội</t>
-  </si>
-  <si>
-    <t>P605C, Cư N105, Nguyễn Phong Sắc, Tổ 7, Dịch Vọng Hậu, Cầu Giấy, Hà Nội</t>
-  </si>
-  <si>
-    <t>143 Yên Lãng, Đống Đa, Hà Nội</t>
-  </si>
-  <si>
-    <t>Tổ 4 - Thịnh Liệt - Hoàng Mai - Hà Nội</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2/199 Phú Viên, Tổ 1, Bồ Đề, Long Biên, Hà Nội </t>
-  </si>
-  <si>
-    <t>Cẩm nhượng, Cẩm xuyên, Hà tĩnh</t>
-  </si>
-  <si>
-    <t>Trung Văn - Nam Từ Liêm - Hà Nội</t>
-  </si>
-  <si>
-    <t>Thôn 3, Phúc Hoà, Phúc Thọ, Hà Nội</t>
-  </si>
-  <si>
-    <t>019186009341</t>
-  </si>
-  <si>
-    <t>8019373151</t>
-  </si>
-  <si>
-    <t>8101391805</t>
-  </si>
-  <si>
-    <t>0103417878</t>
-  </si>
-  <si>
-    <t>0103413841</t>
-  </si>
-  <si>
-    <t>8327096826</t>
-  </si>
-  <si>
-    <t>8026501206</t>
-  </si>
-  <si>
-    <t>8009385976</t>
-  </si>
-  <si>
-    <t>8012846722</t>
-  </si>
-  <si>
-    <t>8009473608</t>
-  </si>
-  <si>
-    <t>8539460058</t>
+    <t>00118200708702</t>
+  </si>
+  <si>
+    <t>02407901654003</t>
+  </si>
+  <si>
+    <t>00118200708703</t>
   </si>
 </sst>
 </file>
@@ -1370,8 +1373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1465,10 +1468,10 @@
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>22</v>
@@ -1478,11 +1481,11 @@
         <v>21</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="12" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="M2" s="12" t="s">
         <v>36</v>
@@ -1491,16 +1494,16 @@
         <v>37</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="P2" s="19">
         <v>8077026742</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="R2" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="S2" s="8"/>
       <c r="T2" s="8"/>
@@ -1515,42 +1518,42 @@
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="12" t="s">
-        <v>60</v>
+        <v>133</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="11" t="s">
         <v>21</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="M3" s="12" t="s">
         <v>38</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>39</v>
       </c>
       <c r="N3" s="11" t="s">
         <v>37</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="P3" s="19">
         <v>8002259299</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="R3" s="11" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="S3" s="7"/>
       <c r="T3" s="7"/>
@@ -1565,10 +1568,10 @@
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="12" t="s">
-        <v>61</v>
+        <v>134</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>22</v>
@@ -1578,29 +1581,29 @@
         <v>21</v>
       </c>
       <c r="J4" s="19" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="13" t="s">
-        <v>40</v>
+        <v>137</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N4" s="11" t="s">
         <v>37</v>
       </c>
       <c r="O4" s="11" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="P4" s="13" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="Q4" s="13" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="R4" s="19" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="S4" s="8"/>
       <c r="T4" s="8"/>
@@ -1615,10 +1618,10 @@
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>22</v>
@@ -1628,29 +1631,29 @@
         <v>21</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="K5" s="5"/>
       <c r="L5" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="N5" s="11" t="s">
         <v>37</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="R5" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
@@ -1665,10 +1668,10 @@
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>22</v>
@@ -1678,29 +1681,29 @@
         <v>21</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M6" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="N6" s="11" t="s">
         <v>37</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="P6" s="13" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="Q6" s="13" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="S6" s="8"/>
       <c r="T6" s="8"/>
@@ -1715,42 +1718,42 @@
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="13" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M7" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="N7" s="11" t="s">
         <v>37</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="P7" s="13" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="Q7" s="13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
@@ -1765,10 +1768,10 @@
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>22</v>
@@ -1778,29 +1781,29 @@
         <v>21</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="M8" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="N8" s="11" t="s">
         <v>37</v>
       </c>
       <c r="O8" s="11" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="P8" s="13" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="Q8" s="13" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="R8" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="S8" s="8"/>
       <c r="T8" s="8"/>
@@ -1815,10 +1818,10 @@
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>22</v>
@@ -1828,29 +1831,29 @@
         <v>21</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="K9" s="5"/>
       <c r="L9" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M9" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N9" s="11" t="s">
         <v>37</v>
       </c>
       <c r="O9" s="11" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="P9" s="13" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="Q9" s="13" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="R9" s="20" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="S9" s="7"/>
       <c r="T9" s="7"/>
@@ -1865,42 +1868,42 @@
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="M10" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="N10" s="11" t="s">
         <v>37</v>
       </c>
       <c r="O10" s="11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="P10" s="13" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="Q10" s="13" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="R10" s="20" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="S10" s="8"/>
       <c r="T10" s="8"/>
@@ -1915,10 +1918,10 @@
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="13" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>22</v>
@@ -1928,29 +1931,29 @@
         <v>21</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="K11" s="5"/>
       <c r="L11" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="M11" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N11" s="11" t="s">
         <v>37</v>
       </c>
       <c r="O11" s="11" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="P11" s="13" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="Q11" s="13" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="R11" s="20" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="S11" s="7"/>
       <c r="T11" s="7"/>
@@ -1965,10 +1968,10 @@
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="13" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>22</v>
@@ -1978,29 +1981,29 @@
         <v>21</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="K12" s="5"/>
       <c r="L12" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M12" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N12" s="11" t="s">
         <v>37</v>
       </c>
       <c r="O12" s="11" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="P12" s="13" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="Q12" s="13" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="R12" s="11" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="S12" s="8"/>
       <c r="T12" s="8"/>
@@ -2015,10 +2018,10 @@
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>22</v>
@@ -2028,29 +2031,29 @@
         <v>21</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="K13" s="5"/>
       <c r="L13" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M13" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="N13" s="11" t="s">
         <v>37</v>
       </c>
       <c r="O13" s="11" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="P13" s="13" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="Q13" s="13" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="R13" s="11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="S13" s="7"/>
       <c r="T13" s="7"/>

</xml_diff>